<commit_message>
docs(README, Minutes, GANTT): update files
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1F9DEC60-C6F7-4D1D-8943-1E5DE98D4A19}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2FC813D-6B6B-4718-977E-8E37494FFC96}"/>
   <bookViews>
-    <workbookView xWindow="18310" yWindow="6090" windowWidth="23350" windowHeight="15830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t xml:space="preserve">PERIODS </t>
   </si>
   <si>
-    <t>Project 16 Planner</t>
-  </si>
-  <si>
     <t>1.2 Group page</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>2.5 GUI design</t>
+  </si>
+  <si>
+    <t>Project 20 Planner</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -722,6 +722,27 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -740,29 +761,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1175,24 +1181,23 @@
   </sheetPr>
   <dimension ref="B1:AM38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AX10" sqref="AX10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.59765625" customWidth="1"/>
-    <col min="2" max="2" width="28.9296875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="11.59765625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.59765625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.58203125" customWidth="1"/>
+    <col min="2" max="2" width="28.9140625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="11.58203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.58203125" style="4" customWidth="1"/>
     <col min="8" max="27" width="4" style="1" customWidth="1"/>
     <col min="28" max="67" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
+    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
       <c r="B1" s="12" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -1200,27 +1205,27 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="51" t="s">
+    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="13">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="55"/>
       <c r="O2" s="15"/>
       <c r="P2" s="22" t="s">
         <v>10</v>
@@ -1235,13 +1240,13 @@
       <c r="V2" s="26"/>
       <c r="W2" s="27"/>
       <c r="Y2" s="17"/>
-      <c r="Z2" s="43" t="s">
+      <c r="Z2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="45"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="52"/>
       <c r="AE2" s="18"/>
       <c r="AF2" s="20" t="s">
         <v>3</v>
@@ -1254,77 +1259,77 @@
       <c r="AL2" s="21"/>
       <c r="AM2" s="21"/>
     </row>
-    <row r="3" spans="2:39" s="10" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="52" t="s">
+    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="49">
+      <c r="J3" s="45">
         <v>44109</v>
       </c>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49">
+      <c r="K3" s="45"/>
+      <c r="L3" s="45">
         <v>44137</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49">
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45">
         <v>44165</v>
       </c>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49">
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45">
         <v>44193</v>
       </c>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="49">
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="45">
         <v>44221</v>
       </c>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49">
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="45"/>
+      <c r="AA3" s="45"/>
+      <c r="AB3" s="45">
         <v>44249</v>
       </c>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49">
+      <c r="AC3" s="45"/>
+      <c r="AD3" s="45"/>
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="45">
         <v>44277</v>
       </c>
-      <c r="AG3" s="49"/>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-    </row>
-    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="53"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="AG3" s="45"/>
+      <c r="AH3" s="45"/>
+      <c r="AI3" s="45"/>
+    </row>
+    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="48"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1410,7 +1415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
@@ -1420,11 +1425,13 @@
       <c r="D5" s="39">
         <v>4</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="57">
+        <v>1</v>
+      </c>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -1434,15 +1441,19 @@
       <c r="D6" s="6">
         <v>4</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
       <c r="G6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -1450,15 +1461,19 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
       <c r="G7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6">
         <v>5</v>
@@ -1466,13 +1481,17 @@
       <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6">
+        <v>7</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="G8" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6">
         <v>6</v>
@@ -1480,13 +1499,17 @@
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="6">
+        <v>6</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
       <c r="G9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="31" t="s">
         <v>14</v>
       </c>
@@ -1496,13 +1519,15 @@
       <c r="D10" s="40">
         <v>3</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="58">
+        <v>6</v>
+      </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
     </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6">
         <v>7</v>
@@ -1510,15 +1535,19 @@
       <c r="D11" s="6">
         <v>2</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="6">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
       <c r="G11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="6">
         <v>7</v>
@@ -1526,15 +1555,17 @@
       <c r="D12" s="6">
         <v>3</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6">
+        <v>6</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="6">
         <v>8</v>
@@ -1542,15 +1573,17 @@
       <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6">
+        <v>7</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6">
         <v>9</v>
@@ -1564,9 +1597,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8">
         <v>9</v>
@@ -1580,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="33" t="s">
         <v>15</v>
       </c>
@@ -1594,7 +1627,7 @@
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
@@ -1610,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="28">
         <v>3.2</v>
       </c>
@@ -1626,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="28">
         <v>3.3</v>
       </c>
@@ -1642,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="28">
         <v>3.4</v>
       </c>
@@ -1658,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="28">
         <v>3.5</v>
       </c>
@@ -1674,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="28">
         <v>3.6</v>
       </c>
@@ -1690,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="28">
         <v>3.7</v>
       </c>
@@ -1706,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="28">
         <v>3.8</v>
       </c>
@@ -1722,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="28">
         <v>3.9</v>
       </c>
@@ -1738,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="28" t="s">
         <v>17</v>
       </c>
@@ -1754,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="34" t="s">
         <v>18</v>
       </c>
@@ -1766,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="28" t="s">
         <v>21</v>
       </c>
@@ -1782,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="28" t="s">
         <v>19</v>
       </c>
@@ -1798,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="28" t="s">
         <v>20</v>
       </c>
@@ -1812,7 +1845,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="35" t="s">
         <v>22</v>
       </c>
@@ -1826,7 +1859,7 @@
       <c r="F31" s="35"/>
       <c r="G31" s="35"/>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="28" t="s">
         <v>23</v>
       </c>
@@ -1840,7 +1873,7 @@
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="28" t="s">
         <v>24</v>
       </c>
@@ -1854,7 +1887,7 @@
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="36" t="s">
         <v>25</v>
       </c>
@@ -1868,7 +1901,7 @@
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="28" t="s">
         <v>26</v>
       </c>
@@ -1882,7 +1915,7 @@
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="28" t="s">
         <v>27</v>
       </c>
@@ -1896,7 +1929,7 @@
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="28" t="s">
         <v>28</v>
       </c>
@@ -1910,7 +1943,7 @@
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="28" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
docs(Technical Reseaarch): add conclusion of TR
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2FC813D-6B6B-4718-977E-8E37494FFC96}"/>
+  <xr:revisionPtr revIDLastSave="595" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D553FF44-D17D-4DA9-A0F7-A918DD86852D}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -171,9 +171,6 @@
     <t>3.1 Create testing structure</t>
   </si>
   <si>
-    <t>3.10 GUI</t>
-  </si>
-  <si>
     <t>4. Reports</t>
   </si>
   <si>
@@ -239,6 +236,33 @@
   </si>
   <si>
     <t>Project 20 Planner</t>
+  </si>
+  <si>
+    <t>3.2 UI for start page</t>
+  </si>
+  <si>
+    <t>3.4 Animate 3 algorithms</t>
+  </si>
+  <si>
+    <t>3.5 Animate 3 algorithms</t>
+  </si>
+  <si>
+    <t>3.6 Tutorial for manual and basic algorithm</t>
+  </si>
+  <si>
+    <t>3.7 Test algorithm correctness</t>
+  </si>
+  <si>
+    <t>3.8 Practice feature</t>
+  </si>
+  <si>
+    <t>3.9 Additional features</t>
+  </si>
+  <si>
+    <t>3.10 Optimise features</t>
+  </si>
+  <si>
+    <t>3.3 Select algorithm feature</t>
   </si>
 </sst>
 </file>
@@ -592,7 +616,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -683,15 +707,9 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -722,6 +740,12 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -764,10 +788,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="15" fillId="8" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="15" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1181,8 +1211,8 @@
   </sheetPr>
   <dimension ref="B1:AM38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AS25" sqref="AS25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1197,7 +1227,7 @@
   <sheetData>
     <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
       <c r="B1" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -1217,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="13">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="53" t="s">
@@ -1279,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="45">
@@ -1419,17 +1449,21 @@
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="39">
-        <v>1</v>
-      </c>
-      <c r="D5" s="39">
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37">
         <v>4</v>
       </c>
-      <c r="E5" s="57">
-        <v>1</v>
-      </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="E5" s="41">
+        <v>1</v>
+      </c>
+      <c r="F5" s="41">
+        <v>8</v>
+      </c>
+      <c r="G5" s="57">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="28" t="s">
@@ -1453,7 +1487,7 @@
     </row>
     <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -1473,7 +1507,7 @@
     </row>
     <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6">
         <v>5</v>
@@ -1484,14 +1518,16 @@
       <c r="E8" s="6">
         <v>7</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6">
+        <v>2</v>
+      </c>
       <c r="G8" s="7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="6">
         <v>6</v>
@@ -1510,24 +1546,28 @@
       </c>
     </row>
     <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="38">
         <v>7</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="38">
         <v>3</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="42">
         <v>6</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="F10" s="42">
+        <v>4</v>
+      </c>
+      <c r="G10" s="58">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6">
         <v>7</v>
@@ -1542,12 +1582,12 @@
         <v>2</v>
       </c>
       <c r="G11" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6">
         <v>7</v>
@@ -1558,14 +1598,16 @@
       <c r="E12" s="6">
         <v>6</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6">
+        <v>3</v>
+      </c>
       <c r="G12" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6">
         <v>8</v>
@@ -1576,14 +1618,16 @@
       <c r="E13" s="6">
         <v>7</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6">
+        <v>3</v>
+      </c>
       <c r="G13" s="7">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6">
         <v>9</v>
@@ -1591,15 +1635,19 @@
       <c r="D14" s="6">
         <v>1</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="6">
+        <v>9</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
       <c r="G14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="8">
         <v>9</v>
@@ -1607,25 +1655,29 @@
       <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="E15" s="6">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6">
+        <v>2</v>
+      </c>
       <c r="G15" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="36">
         <v>10</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="36">
         <v>12</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="28" t="s">
@@ -1644,8 +1696,8 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="28">
-        <v>3.2</v>
+      <c r="B18" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="6">
         <v>11</v>
@@ -1660,8 +1712,8 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="28">
-        <v>3.3</v>
+      <c r="B19" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="6">
         <v>12</v>
@@ -1676,8 +1728,8 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="28">
-        <v>3.4</v>
+      <c r="B20" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="6">
         <v>13</v>
@@ -1692,8 +1744,8 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="28">
-        <v>3.5</v>
+      <c r="B21" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="6">
         <v>15</v>
@@ -1708,8 +1760,8 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="28">
-        <v>3.6</v>
+      <c r="B22" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="C22" s="6">
         <v>16</v>
@@ -1724,8 +1776,8 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="28">
-        <v>3.7</v>
+      <c r="B23" s="28" t="s">
+        <v>43</v>
       </c>
       <c r="C23" s="6">
         <v>18</v>
@@ -1740,8 +1792,8 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="28">
-        <v>3.8</v>
+      <c r="B24" s="28" t="s">
+        <v>44</v>
       </c>
       <c r="C24" s="6">
         <v>19</v>
@@ -1756,8 +1808,8 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="28">
-        <v>3.9</v>
+      <c r="B25" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="6">
         <v>20</v>
@@ -1773,7 +1825,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="28" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C26" s="6">
         <v>21</v>
@@ -1788,20 +1840,18 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34">
-        <v>0</v>
-      </c>
+      <c r="B27" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="6">
         <v>5</v>
@@ -1809,15 +1859,19 @@
       <c r="D28" s="6">
         <v>4</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="E28" s="6">
+        <v>5</v>
+      </c>
+      <c r="F28" s="6">
+        <v>5</v>
+      </c>
       <c r="G28" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="6">
         <v>22</v>
@@ -1833,7 +1887,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="6">
         <v>22</v>
@@ -1843,25 +1897,27 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
+      <c r="G30" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="41">
+      <c r="B31" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="41">
+      <c r="C31" s="39">
+        <v>21</v>
+      </c>
+      <c r="D31" s="39">
         <v>6</v>
       </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="39"/>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="6">
         <v>21</v>
@@ -1871,11 +1927,13 @@
       </c>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
+      <c r="G32" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="6">
         <v>24</v>
@@ -1885,25 +1943,27 @@
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="G33" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="42">
+      <c r="B34" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="40">
         <v>21</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="40">
         <v>8</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="60"/>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="6">
         <v>21</v>
@@ -1913,11 +1973,13 @@
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
+      <c r="G35" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="6">
         <v>23</v>
@@ -1927,11 +1989,13 @@
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
+      <c r="G36" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="6">
         <v>25</v>
@@ -1941,11 +2005,13 @@
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
+      <c r="G37" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="6">
         <v>28</v>
@@ -1955,7 +2021,9 @@
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
+      <c r="G38" s="59">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
docs(Minutes): add minutes of 28th meeting
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="595" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D553FF44-D17D-4DA9-A0F7-A918DD86852D}"/>
+  <xr:revisionPtr revIDLastSave="723" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7CAD489E-0834-A548-A2BD-ABD6368B9610}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26500" yWindow="4580" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -238,18 +237,6 @@
     <t>Project 20 Planner</t>
   </si>
   <si>
-    <t>3.2 UI for start page</t>
-  </si>
-  <si>
-    <t>3.4 Animate 3 algorithms</t>
-  </si>
-  <si>
-    <t>3.5 Animate 3 algorithms</t>
-  </si>
-  <si>
-    <t>3.6 Tutorial for manual and basic algorithm</t>
-  </si>
-  <si>
     <t>3.7 Test algorithm correctness</t>
   </si>
   <si>
@@ -262,14 +249,55 @@
     <t>3.10 Optimise features</t>
   </si>
   <si>
-    <t>3.3 Select algorithm feature</t>
+    <t>3.5 make swap animation</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6 Bubble sort algorithm</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.4 UI for start page &amp; subpages</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.7 Router feat &amp; local storage</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3 Make basic components</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2 Learn related knowledge</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.8 Animate 2 algorithms (SI)</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.9 Help and setting</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.10 Correctness proposal</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.11 improve ui with electron</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.12 animate merge and heap</t>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -304,12 +332,14 @@
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="7"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -383,6 +413,13 @@
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="14">
@@ -746,6 +783,18 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="15" fillId="8" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -786,18 +835,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="8" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -807,20 +844,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1209,23 +1246,23 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AM38"/>
+  <dimension ref="B1:AM44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AS25" sqref="AS25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="28.9140625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.58203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.58203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="11.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="27" width="4" style="1" customWidth="1"/>
     <col min="28" max="67" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
+    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1">
       <c r="B1" s="12" t="s">
         <v>38</v>
       </c>
@@ -1235,14 +1272,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="46" t="s">
+    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1250,12 +1287,12 @@
         <v>9</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="53" t="s">
+      <c r="K2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="59"/>
       <c r="O2" s="15"/>
       <c r="P2" s="22" t="s">
         <v>10</v>
@@ -1270,13 +1307,13 @@
       <c r="V2" s="26"/>
       <c r="W2" s="27"/>
       <c r="Y2" s="17"/>
-      <c r="Z2" s="50" t="s">
+      <c r="Z2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="52"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="56"/>
       <c r="AE2" s="18"/>
       <c r="AF2" s="20" t="s">
         <v>3</v>
@@ -1289,77 +1326,77 @@
       <c r="AL2" s="21"/>
       <c r="AM2" s="21"/>
     </row>
-    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="47" t="s">
+    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1">
+      <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="47" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="9"/>
-      <c r="J3" s="45">
+      <c r="J3" s="49">
         <v>44109</v>
       </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45">
+      <c r="K3" s="49"/>
+      <c r="L3" s="49">
         <v>44137</v>
       </c>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45">
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49">
         <v>44165</v>
       </c>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45">
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49">
         <v>44193</v>
       </c>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="45">
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="49">
         <v>44221</v>
       </c>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45">
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49">
         <v>44249</v>
       </c>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45">
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49">
         <v>44277</v>
       </c>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
-    </row>
-    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="48"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+    </row>
+    <row r="4" spans="2:39" ht="15.75" customHeight="1">
+      <c r="B4" s="52"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1445,7 +1482,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:39" ht="30" customHeight="1">
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
@@ -1461,11 +1498,11 @@
       <c r="F5" s="41">
         <v>8</v>
       </c>
-      <c r="G5" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G5" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:39" ht="30" customHeight="1">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -1485,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:39" ht="30" customHeight="1">
       <c r="B7" s="28" t="s">
         <v>30</v>
       </c>
@@ -1505,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:39" ht="30" customHeight="1">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -1525,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:39" ht="30" customHeight="1">
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -1545,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:39" ht="30" customHeight="1">
       <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
@@ -1561,11 +1598,11 @@
       <c r="F10" s="42">
         <v>4</v>
       </c>
-      <c r="G10" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G10" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:39" ht="30" customHeight="1">
       <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:39" ht="30" customHeight="1">
       <c r="B12" s="28" t="s">
         <v>34</v>
       </c>
@@ -1605,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:39" ht="30" customHeight="1">
       <c r="B13" s="28" t="s">
         <v>35</v>
       </c>
@@ -1625,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:39" ht="30" customHeight="1">
       <c r="B14" s="28" t="s">
         <v>36</v>
       </c>
@@ -1645,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:39" ht="30" customHeight="1">
       <c r="B15" s="28" t="s">
         <v>37</v>
       </c>
@@ -1665,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:39" ht="30" customHeight="1">
       <c r="B16" s="31" t="s">
         <v>15</v>
       </c>
@@ -1679,7 +1716,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="36"/>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:7" ht="30" customHeight="1">
       <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
@@ -1689,195 +1726,233 @@
       <c r="D17" s="6">
         <v>2</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="E17" s="6">
+        <v>14</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
       <c r="G17" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1">
       <c r="B18" s="28" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C18" s="6">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D18" s="6">
         <v>2</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="6">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
       <c r="G18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1">
       <c r="B19" s="28" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="6">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D19" s="6">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
+        <v>16</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
       <c r="G19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1">
       <c r="B20" s="28" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C20" s="6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D20" s="6">
-        <v>2</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>16</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
       <c r="G20" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1">
       <c r="B21" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C21" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" s="6">
-        <v>2</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>16</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
       <c r="G21" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1">
       <c r="B22" s="28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C22" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D22" s="6">
-        <v>2</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>17</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1</v>
+      </c>
       <c r="G22" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1">
       <c r="B23" s="28" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C23" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="6">
-        <v>3</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="6">
+        <v>17</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
       <c r="G23" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="28" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D24" s="6">
-        <v>2</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>17</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
       <c r="G24" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1">
       <c r="B25" s="28" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C25" s="6">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D25" s="6">
-        <v>2</v>
-      </c>
-      <c r="E25" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <v>17</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30" customHeight="1">
       <c r="B26" s="28" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C26" s="6">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6">
+        <v>18</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1">
+      <c r="B27" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="6">
+        <v>18</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6">
+        <v>18</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="2:7" ht="30" customHeight="1">
       <c r="B28" s="28" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C28" s="6">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D28" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E28" s="6">
-        <v>5</v>
-      </c>
-      <c r="F28" s="6">
-        <v>5</v>
-      </c>
-      <c r="G28" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="2:7" ht="30" customHeight="1">
       <c r="B29" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="6">
         <v>18</v>
       </c>
-      <c r="C29" s="6">
-        <v>22</v>
-      </c>
       <c r="D29" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -1885,15 +1960,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:7" ht="30" customHeight="1">
       <c r="B30" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="6">
         <v>19</v>
       </c>
-      <c r="C30" s="6">
-        <v>22</v>
-      </c>
       <c r="D30" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -1901,127 +1976,221 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="39">
-        <v>21</v>
-      </c>
-      <c r="D31" s="39">
-        <v>6</v>
-      </c>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:7" ht="30" customHeight="1">
+      <c r="B31" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="6">
+        <v>20</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1">
       <c r="B32" s="28" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C32" s="6">
         <v>21</v>
       </c>
       <c r="D32" s="6">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1">
+      <c r="B33" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="35"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="35"/>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1">
+      <c r="B34" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="6">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6">
+        <v>4</v>
+      </c>
+      <c r="E34" s="6">
+        <v>5</v>
+      </c>
+      <c r="F34" s="6">
+        <v>5</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1">
+      <c r="B35" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="6">
+        <v>22</v>
+      </c>
+      <c r="D35" s="6">
+        <v>6</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1">
+      <c r="B36" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="6">
+        <v>22</v>
+      </c>
+      <c r="D36" s="6">
+        <v>7</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1">
+      <c r="B37" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="39">
+        <v>21</v>
+      </c>
+      <c r="D37" s="39">
+        <v>6</v>
+      </c>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="39"/>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1">
+      <c r="B38" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="6">
+        <v>21</v>
+      </c>
+      <c r="D38" s="6">
         <v>3</v>
-      </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="6">
-        <v>24</v>
-      </c>
-      <c r="D33" s="6">
-        <v>3</v>
-      </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="40">
-        <v>21</v>
-      </c>
-      <c r="D34" s="40">
-        <v>8</v>
-      </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="60"/>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="6">
-        <v>21</v>
-      </c>
-      <c r="D35" s="6">
-        <v>3</v>
-      </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="6">
-        <v>23</v>
-      </c>
-      <c r="D36" s="6">
-        <v>3</v>
-      </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="6">
-        <v>25</v>
-      </c>
-      <c r="D37" s="6">
-        <v>3</v>
-      </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="6">
-        <v>28</v>
-      </c>
-      <c r="D38" s="6">
-        <v>1</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
-      <c r="G38" s="59">
+      <c r="G38" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1">
+      <c r="B39" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="6">
+        <v>24</v>
+      </c>
+      <c r="D39" s="6">
+        <v>3</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1">
+      <c r="B40" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="40">
+        <v>21</v>
+      </c>
+      <c r="D40" s="40">
+        <v>8</v>
+      </c>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="46"/>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1">
+      <c r="B41" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="6">
+        <v>21</v>
+      </c>
+      <c r="D41" s="6">
+        <v>3</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1">
+      <c r="B42" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="6">
+        <v>23</v>
+      </c>
+      <c r="D42" s="6">
+        <v>3</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1">
+      <c r="B43" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="6">
+        <v>25</v>
+      </c>
+      <c r="D43" s="6">
+        <v>3</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1">
+      <c r="B44" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="6">
+        <v>28</v>
+      </c>
+      <c r="D44" s="6">
+        <v>1</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="45">
         <v>0</v>
       </c>
     </row>
@@ -2044,7 +2213,8 @@
     <mergeCell ref="T3:W3"/>
     <mergeCell ref="J3:K3"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:AI38">
+  <phoneticPr fontId="16" type="noConversion"/>
+  <conditionalFormatting sqref="H5:AI44">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2070,7 +2240,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:BO39">
+  <conditionalFormatting sqref="B45:BO45">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs(Minutes): add minutes for 29th meeting
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7CAD489E-0834-A548-A2BD-ABD6368B9610}"/>
+  <xr:revisionPtr revIDLastSave="732" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8F5D2BD0-0E5A-A84B-A430-A6970B29E648}"/>
   <bookViews>
-    <workbookView xWindow="26500" yWindow="4580" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="4400" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1248,8 +1248,8 @@
   </sheetPr>
   <dimension ref="B1:AM44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
@@ -1889,7 +1889,9 @@
       <c r="E25" s="6">
         <v>17</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
       <c r="G25" s="7">
         <v>0.8</v>
       </c>
@@ -1907,7 +1909,9 @@
       <c r="E26" s="6">
         <v>18</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="6">
+        <v>1</v>
+      </c>
       <c r="G26" s="7">
         <v>0.8</v>
       </c>
@@ -1925,8 +1929,12 @@
       <c r="E27" s="6">
         <v>18</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1">
       <c r="B28" s="28" t="s">
@@ -1942,7 +1950,9 @@
         <v>18</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
+      <c r="G28" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1">
       <c r="B29" s="28" t="s">

</xml_diff>

<commit_message>
docs(Images): update images of 0212
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="732" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8F5D2BD0-0E5A-A84B-A430-A6970B29E648}"/>
+  <xr:revisionPtr revIDLastSave="736" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{602603AE-D021-4549-96E3-BE26DD68B926}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="4400" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="49960" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1248,8 +1248,8 @@
   </sheetPr>
   <dimension ref="B1:AM44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="94" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AT30" sqref="AT30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
@@ -1893,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1">
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1">
@@ -1949,9 +1949,11 @@
       <c r="E28" s="6">
         <v>18</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
       <c r="G28" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1">

</xml_diff>

<commit_message>
docs(GANTT): update gantt chart to week 21
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="736" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{602603AE-D021-4549-96E3-BE26DD68B926}"/>
+  <xr:revisionPtr revIDLastSave="764" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{562F929E-5BCD-434B-85B9-B1A77A054E36}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="460" windowWidth="49960" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24480" yWindow="4600" windowWidth="30580" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -290,6 +290,18 @@
   </si>
   <si>
     <t>3.12 animate merge and heap</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.13 refactor previous work</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.14 design correctness part</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.15 correctness tutorial</t>
     <phoneticPr fontId="16" type="noConversion"/>
   </si>
 </sst>
@@ -1246,10 +1258,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AM44"/>
+  <dimension ref="B1:AM47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="94" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AT30" sqref="AT30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="94" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
@@ -1958,107 +1970,121 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1">
       <c r="B29" s="28" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C29" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D29" s="6">
-        <v>3</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="6">
+        <v>20</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
       <c r="G29" s="7">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1">
       <c r="B30" s="28" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C30" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <v>20</v>
+      </c>
+      <c r="F30" s="6">
         <v>2</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
       <c r="G30" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1">
       <c r="B31" s="28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C31" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" s="6">
-        <v>2</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E31" s="6">
+        <v>21</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1">
       <c r="B32" s="28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C32" s="6">
         <v>21</v>
       </c>
       <c r="D32" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="F32" s="6">
+        <v>2</v>
+      </c>
       <c r="G32" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1">
-      <c r="B33" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="35"/>
+      <c r="B33" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="6">
+        <v>19</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1">
       <c r="B34" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="6">
         <v>20</v>
       </c>
-      <c r="C34" s="6">
-        <v>5</v>
-      </c>
       <c r="D34" s="6">
-        <v>4</v>
-      </c>
-      <c r="E34" s="6">
-        <v>5</v>
-      </c>
-      <c r="F34" s="6">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
       <c r="G34" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1">
       <c r="B35" s="28" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C35" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -2067,84 +2093,84 @@
       </c>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1">
-      <c r="B36" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="6">
-        <v>22</v>
-      </c>
-      <c r="D36" s="6">
-        <v>7</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7">
-        <v>0</v>
-      </c>
+      <c r="B36" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="35"/>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1">
-      <c r="B37" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="39">
-        <v>21</v>
-      </c>
-      <c r="D37" s="39">
-        <v>6</v>
-      </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="39"/>
+      <c r="B37" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="6">
+        <v>5</v>
+      </c>
+      <c r="D37" s="6">
+        <v>4</v>
+      </c>
+      <c r="E37" s="6">
+        <v>5</v>
+      </c>
+      <c r="F37" s="6">
+        <v>5</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1">
       <c r="B38" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="6">
         <v>22</v>
       </c>
-      <c r="C38" s="6">
-        <v>21</v>
-      </c>
       <c r="D38" s="6">
-        <v>3</v>
-      </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="45">
+        <v>6</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1">
       <c r="B39" s="28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C39" s="6">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D39" s="6">
-        <v>3</v>
-      </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="45">
+        <v>7</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="30" customHeight="1">
-      <c r="B40" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="40">
+      <c r="B40" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="40">
-        <v>8</v>
-      </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="46"/>
+      <c r="C40" s="39">
+        <v>21</v>
+      </c>
+      <c r="D40" s="39">
+        <v>6</v>
+      </c>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="39"/>
     </row>
     <row r="41" spans="2:7" ht="30" customHeight="1">
       <c r="B41" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C41" s="6">
         <v>21</v>
@@ -2160,10 +2186,10 @@
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1">
       <c r="B42" s="28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C42" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D42" s="6">
         <v>3</v>
@@ -2175,34 +2201,80 @@
       </c>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C43" s="6">
-        <v>25</v>
-      </c>
-      <c r="D43" s="6">
-        <v>3</v>
-      </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="45">
-        <v>0</v>
-      </c>
+      <c r="B43" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="40">
+        <v>21</v>
+      </c>
+      <c r="D43" s="40">
+        <v>8</v>
+      </c>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="46"/>
     </row>
     <row r="44" spans="2:7" ht="30" customHeight="1">
       <c r="B44" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C44" s="6">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D44" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
       <c r="G44" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30" customHeight="1">
+      <c r="B45" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="6">
+        <v>23</v>
+      </c>
+      <c r="D45" s="6">
+        <v>3</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="30" customHeight="1">
+      <c r="B46" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="6">
+        <v>25</v>
+      </c>
+      <c r="D46" s="6">
+        <v>3</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1">
+      <c r="B47" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="6">
+        <v>28</v>
+      </c>
+      <c r="D47" s="6">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="45">
         <v>0</v>
       </c>
     </row>
@@ -2226,7 +2298,7 @@
     <mergeCell ref="J3:K3"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
-  <conditionalFormatting sqref="H5:AI44">
+  <conditionalFormatting sqref="H5:AI47">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2252,7 +2324,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45:BO45">
+  <conditionalFormatting sqref="B48:BO48">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs(gantt): update gantt and images
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="764" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{562F929E-5BCD-434B-85B9-B1A77A054E36}"/>
+  <xr:revisionPtr revIDLastSave="788" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5F43EFB5-2B96-4CA4-8A38-DA5DF992C269}"/>
   <bookViews>
-    <workbookView xWindow="24480" yWindow="4600" windowWidth="30580" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -303,6 +303,12 @@
   <si>
     <t>3.15 correctness tutorial</t>
     <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.16 Tutorial design</t>
+  </si>
+  <si>
+    <t>3.17 Tutorial pages</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Corbel"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -856,20 +862,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1258,13 +1264,13 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AM47"/>
+  <dimension ref="B1:AM49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="94" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
@@ -1296,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="13">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="57" t="s">
@@ -1961,11 +1967,9 @@
       <c r="E28" s="6">
         <v>18</v>
       </c>
-      <c r="F28" s="6">
-        <v>1</v>
-      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1">
@@ -1985,7 +1989,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1">
@@ -2021,70 +2025,74 @@
       <c r="E31" s="6">
         <v>21</v>
       </c>
-      <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="7"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1">
       <c r="B32" s="28" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C32" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32" s="6">
-        <v>3</v>
-      </c>
-      <c r="E32" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="6">
+        <v>22</v>
+      </c>
       <c r="F32" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1">
       <c r="B33" s="28" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C33" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D33" s="6">
         <v>2</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="6">
+        <v>23</v>
+      </c>
       <c r="F33" s="6"/>
-      <c r="G33" s="7">
-        <v>0</v>
-      </c>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1">
       <c r="B34" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D34" s="6">
+        <v>3</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6">
         <v>2</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
       <c r="G34" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1">
       <c r="B35" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="6">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D35" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -2093,133 +2101,137 @@
       </c>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1">
-      <c r="B36" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="35"/>
+      <c r="B36" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="6">
+        <v>20</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1">
       <c r="B37" s="28" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C37" s="6">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D37" s="6">
-        <v>4</v>
-      </c>
-      <c r="E37" s="6">
-        <v>5</v>
-      </c>
-      <c r="F37" s="6">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1">
-      <c r="B38" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="6">
-        <v>22</v>
-      </c>
-      <c r="D38" s="6">
-        <v>6</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="7">
-        <v>0</v>
-      </c>
+      <c r="B38" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="35"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="35"/>
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1">
       <c r="B39" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C39" s="6">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6">
+        <v>4</v>
+      </c>
+      <c r="E39" s="6">
+        <v>5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>5</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1">
+      <c r="B40" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="6">
         <v>22</v>
       </c>
-      <c r="D39" s="6">
-        <v>7</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1">
-      <c r="B40" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="39">
-        <v>21</v>
-      </c>
-      <c r="D40" s="39">
+      <c r="D40" s="6">
         <v>6</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="39"/>
+      <c r="E40" s="6">
+        <v>22</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="41" spans="2:7" ht="30" customHeight="1">
       <c r="B41" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="6">
         <v>22</v>
       </c>
-      <c r="C41" s="6">
+      <c r="D41" s="6">
+        <v>7</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1">
+      <c r="B42" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="6">
+      <c r="C42" s="39">
+        <v>21</v>
+      </c>
+      <c r="D42" s="39">
+        <v>6</v>
+      </c>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="39"/>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1">
+      <c r="B43" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="6">
+        <v>21</v>
+      </c>
+      <c r="D43" s="6">
         <v>3</v>
       </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="45">
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="45">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1">
-      <c r="B42" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="6">
-        <v>24</v>
-      </c>
-      <c r="D42" s="6">
-        <v>3</v>
-      </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="40">
-        <v>21</v>
-      </c>
-      <c r="D43" s="40">
-        <v>8</v>
-      </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="46"/>
     </row>
     <row r="44" spans="2:7" ht="30" customHeight="1">
       <c r="B44" s="28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C44" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D44" s="6">
         <v>3</v>
@@ -2231,27 +2243,25 @@
       </c>
     </row>
     <row r="45" spans="2:7" ht="30" customHeight="1">
-      <c r="B45" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="6">
-        <v>23</v>
-      </c>
-      <c r="D45" s="6">
-        <v>3</v>
-      </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="45">
-        <v>0</v>
-      </c>
+      <c r="B45" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="40">
+        <v>21</v>
+      </c>
+      <c r="D45" s="40">
+        <v>8</v>
+      </c>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="46"/>
     </row>
     <row r="46" spans="2:7" ht="30" customHeight="1">
       <c r="B46" s="28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C46" s="6">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D46" s="6">
         <v>3</v>
@@ -2264,17 +2274,49 @@
     </row>
     <row r="47" spans="2:7" ht="30" customHeight="1">
       <c r="B47" s="28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C47" s="6">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D47" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="28"/>
       <c r="G47" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="30" customHeight="1">
+      <c r="B48" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="6">
+        <v>25</v>
+      </c>
+      <c r="D48" s="6">
+        <v>3</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="30" customHeight="1">
+      <c r="B49" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="6">
+        <v>28</v>
+      </c>
+      <c r="D49" s="6">
+        <v>1</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="45">
         <v>0</v>
       </c>
     </row>
@@ -2298,7 +2340,7 @@
     <mergeCell ref="J3:K3"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
-  <conditionalFormatting sqref="H5:AI47">
+  <conditionalFormatting sqref="H5:AI49">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2324,7 +2366,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48:BO48">
+  <conditionalFormatting sqref="B50:BO50">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs(readme): update timeline and gantt
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colin/OneDrive/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="788" documentId="8_{65675DDE-D1E2-4E9F-9F72-1EAB5D416229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5F43EFB5-2B96-4CA4-8A38-DA5DF992C269}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="2660" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -310,12 +310,28 @@
   <si>
     <t>3.17 Tutorial pages</t>
   </si>
+  <si>
+    <t>3.18 Procedure imple</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.19 Improve transition anime</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.20 Refactor previous work</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.21 Correctness proof</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -862,20 +878,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1264,13 +1280,13 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AM49"/>
+  <dimension ref="B1:AM53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="89" zoomScaleNormal="66" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
@@ -1280,7 +1296,7 @@
     <col min="28" max="67" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1">
+    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="12" t="s">
         <v>38</v>
       </c>
@@ -1290,7 +1306,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1">
+    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="50" t="s">
         <v>4</v>
       </c>
@@ -1344,7 +1360,7 @@
       <c r="AL2" s="21"/>
       <c r="AM2" s="21"/>
     </row>
-    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1">
+    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1424,7 @@
       <c r="AH3" s="49"/>
       <c r="AI3" s="49"/>
     </row>
-    <row r="4" spans="2:39" ht="15.75" customHeight="1">
+    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="52"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -1500,7 +1516,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="30" customHeight="1">
+    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
@@ -1520,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:39" ht="30" customHeight="1">
+    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -1540,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="30" customHeight="1">
+    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
         <v>30</v>
       </c>
@@ -1560,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="30" customHeight="1">
+    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -1580,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="30" customHeight="1">
+    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -1600,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="30" customHeight="1">
+    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1">
+    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
@@ -1640,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="30" customHeight="1">
+    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="28" t="s">
         <v>34</v>
       </c>
@@ -1660,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:39" ht="30" customHeight="1">
+    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>35</v>
       </c>
@@ -1680,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="30" customHeight="1">
+    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="28" t="s">
         <v>36</v>
       </c>
@@ -1700,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="30" customHeight="1">
+    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="28" t="s">
         <v>37</v>
       </c>
@@ -1720,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="30" customHeight="1">
+    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
         <v>15</v>
       </c>
@@ -1730,11 +1746,13 @@
       <c r="D16" s="36">
         <v>12</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="36">
+        <v>14</v>
+      </c>
       <c r="F16" s="31"/>
       <c r="G16" s="36"/>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
@@ -1754,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="s">
         <v>48</v>
       </c>
@@ -1774,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="28" t="s">
         <v>47</v>
       </c>
@@ -1794,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="28" t="s">
         <v>45</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="28" t="s">
         <v>43</v>
       </c>
@@ -1834,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>44</v>
       </c>
@@ -1854,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>46</v>
       </c>
@@ -1874,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>49</v>
       </c>
@@ -1894,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="28" t="s">
         <v>50</v>
       </c>
@@ -1914,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="28" t="s">
         <v>51</v>
       </c>
@@ -1934,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="28" t="s">
         <v>52</v>
       </c>
@@ -1954,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="28" t="s">
         <v>53</v>
       </c>
@@ -1967,12 +1985,14 @@
       <c r="E28" s="6">
         <v>18</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="6">
+        <v>4</v>
+      </c>
       <c r="G28" s="7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="28" t="s">
         <v>54</v>
       </c>
@@ -1992,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="28" t="s">
         <v>55</v>
       </c>
@@ -2012,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="28" t="s">
         <v>56</v>
       </c>
@@ -2027,10 +2047,10 @@
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="28" t="s">
         <v>57</v>
       </c>
@@ -2050,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="28" t="s">
         <v>58</v>
       </c>
@@ -2064,131 +2084,133 @@
         <v>23</v>
       </c>
       <c r="F33" s="6"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1">
+      <c r="G33" s="7">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="28" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C34" s="6">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D34" s="6">
-        <v>3</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6">
         <v>2</v>
       </c>
+      <c r="E34" s="6">
+        <v>23</v>
+      </c>
+      <c r="F34" s="6"/>
       <c r="G34" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="28" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C35" s="6">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D35" s="6">
-        <v>2</v>
-      </c>
-      <c r="E35" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="6">
+        <v>24</v>
+      </c>
       <c r="F35" s="6"/>
-      <c r="G35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1">
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="28" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C36" s="6">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D36" s="6">
-        <v>2</v>
-      </c>
-      <c r="E36" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E36" s="6">
+        <v>24</v>
+      </c>
       <c r="F36" s="6"/>
-      <c r="G36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1">
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="28" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C37" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D37" s="6">
         <v>1</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-      <c r="G37" s="7">
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="6">
+        <v>21</v>
+      </c>
+      <c r="D38" s="6">
+        <v>3</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6">
+        <v>2</v>
+      </c>
+      <c r="G38" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1">
-      <c r="B38" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="35"/>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="6">
+        <v>19</v>
+      </c>
+      <c r="D39" s="6">
+        <v>2</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="6">
         <v>20</v>
       </c>
-      <c r="C39" s="6">
-        <v>5</v>
-      </c>
-      <c r="D39" s="6">
-        <v>4</v>
-      </c>
-      <c r="E39" s="6">
-        <v>5</v>
-      </c>
-      <c r="F39" s="6">
-        <v>5</v>
-      </c>
-      <c r="G39" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1">
-      <c r="B40" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="6">
-        <v>22</v>
-      </c>
       <c r="D40" s="6">
-        <v>6</v>
-      </c>
-      <c r="E40" s="6">
-        <v>22</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="30" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="28" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C41" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D41" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -2196,88 +2218,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1">
-      <c r="B42" s="33" t="s">
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="35"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="35"/>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="6">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6">
+        <v>4</v>
+      </c>
+      <c r="E43" s="6">
+        <v>5</v>
+      </c>
+      <c r="F43" s="6">
+        <v>5</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="6">
+        <v>22</v>
+      </c>
+      <c r="D44" s="6">
+        <v>6</v>
+      </c>
+      <c r="E44" s="6">
+        <v>22</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="6">
+        <v>22</v>
+      </c>
+      <c r="D45" s="6">
+        <v>7</v>
+      </c>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="39">
+      <c r="C46" s="39">
         <v>21</v>
       </c>
-      <c r="D42" s="39">
+      <c r="D46" s="39">
         <v>6</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="39"/>
-    </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="28" t="s">
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="39"/>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C47" s="6">
         <v>21</v>
-      </c>
-      <c r="D43" s="6">
-        <v>3</v>
-      </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="30" customHeight="1">
-      <c r="B44" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="6">
-        <v>24</v>
-      </c>
-      <c r="D44" s="6">
-        <v>3</v>
-      </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1">
-      <c r="B45" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="40">
-        <v>21</v>
-      </c>
-      <c r="D45" s="40">
-        <v>8</v>
-      </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="46"/>
-    </row>
-    <row r="46" spans="2:7" ht="30" customHeight="1">
-      <c r="B46" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="6">
-        <v>21</v>
-      </c>
-      <c r="D46" s="6">
-        <v>3</v>
-      </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1">
-      <c r="B47" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="6">
-        <v>23</v>
       </c>
       <c r="D47" s="6">
         <v>3</v>
@@ -2288,12 +2312,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" ht="30" customHeight="1">
+    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C48" s="6">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" s="6">
         <v>3</v>
@@ -2304,19 +2328,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1">
-      <c r="B49" s="28" t="s">
+    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="40">
+        <v>21</v>
+      </c>
+      <c r="D49" s="40">
+        <v>8</v>
+      </c>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="46"/>
+    </row>
+    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="6">
+        <v>21</v>
+      </c>
+      <c r="D50" s="6">
+        <v>3</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="6">
+        <v>23</v>
+      </c>
+      <c r="D51" s="6">
+        <v>3</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="6">
+        <v>25</v>
+      </c>
+      <c r="D52" s="6">
+        <v>3</v>
+      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C53" s="6">
         <v>28</v>
       </c>
-      <c r="D49" s="6">
-        <v>1</v>
-      </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="45">
+      <c r="D53" s="6">
+        <v>1</v>
+      </c>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="45">
         <v>0</v>
       </c>
     </row>
@@ -2340,7 +2426,7 @@
     <mergeCell ref="J3:K3"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
-  <conditionalFormatting sqref="H5:AI49">
+  <conditionalFormatting sqref="H5:AI53">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2366,7 +2452,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:BO50">
+  <conditionalFormatting sqref="B54:BO54">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs(image): update snapshot of gantt and kanban
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colin/OneDrive/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C07E049D-7210-4BC1-8A06-9A03FFD2ACFA}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="2660" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -331,7 +331,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -878,20 +878,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1282,11 +1282,11 @@
   </sheetPr>
   <dimension ref="B1:AM53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="89" zoomScaleNormal="66" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="61" zoomScaleNormal="61" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BK26" sqref="BK26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
@@ -1296,7 +1296,7 @@
     <col min="28" max="67" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1">
       <c r="B1" s="12" t="s">
         <v>38</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="B2" s="50" t="s">
         <v>4</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="13">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="57" t="s">
@@ -1360,7 +1360,7 @@
       <c r="AL2" s="21"/>
       <c r="AM2" s="21"/>
     </row>
-    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1">
       <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="AH3" s="49"/>
       <c r="AI3" s="49"/>
     </row>
-    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:39" ht="15.75" customHeight="1">
       <c r="B4" s="52"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -1516,7 +1516,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:39" ht="30" customHeight="1">
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:39" ht="30" customHeight="1">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:39" ht="30" customHeight="1">
       <c r="B7" s="28" t="s">
         <v>30</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:39" ht="30" customHeight="1">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:39" ht="30" customHeight="1">
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:39" ht="30" customHeight="1">
       <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:39" ht="30" customHeight="1">
       <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:39" ht="30" customHeight="1">
       <c r="B12" s="28" t="s">
         <v>34</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:39" ht="30" customHeight="1">
       <c r="B13" s="28" t="s">
         <v>35</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:39" ht="30" customHeight="1">
       <c r="B14" s="28" t="s">
         <v>36</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:39" ht="30" customHeight="1">
       <c r="B15" s="28" t="s">
         <v>37</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:39" ht="30" customHeight="1">
       <c r="B16" s="31" t="s">
         <v>15</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="36"/>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="30" customHeight="1">
       <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="30" customHeight="1">
       <c r="B18" s="28" t="s">
         <v>48</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="30" customHeight="1">
       <c r="B19" s="28" t="s">
         <v>47</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="30" customHeight="1">
       <c r="B20" s="28" t="s">
         <v>45</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="30" customHeight="1">
       <c r="B21" s="28" t="s">
         <v>43</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="30" customHeight="1">
       <c r="B22" s="28" t="s">
         <v>44</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="30" customHeight="1">
       <c r="B23" s="28" t="s">
         <v>46</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="28" t="s">
         <v>49</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="30" customHeight="1">
       <c r="B25" s="28" t="s">
         <v>50</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="30" customHeight="1">
       <c r="B26" s="28" t="s">
         <v>51</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="30" customHeight="1">
       <c r="B27" s="28" t="s">
         <v>52</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="30" customHeight="1">
       <c r="B28" s="28" t="s">
         <v>53</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="30" customHeight="1">
       <c r="B29" s="28" t="s">
         <v>54</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" ht="30" customHeight="1">
       <c r="B30" s="28" t="s">
         <v>55</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" ht="30" customHeight="1">
       <c r="B31" s="28" t="s">
         <v>56</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" ht="30" customHeight="1">
       <c r="B32" s="28" t="s">
         <v>57</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="30" customHeight="1">
       <c r="B33" s="28" t="s">
         <v>58</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" ht="30" customHeight="1">
       <c r="B34" s="28" t="s">
         <v>59</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" ht="30" customHeight="1">
       <c r="B35" s="28" t="s">
         <v>60</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" ht="30" customHeight="1">
       <c r="B36" s="28" t="s">
         <v>61</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" ht="30" customHeight="1">
       <c r="B37" s="28" t="s">
         <v>62</v>
       </c>
@@ -2152,7 +2152,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="30" customHeight="1">
       <c r="B38" s="28" t="s">
         <v>39</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="30" customHeight="1">
       <c r="B39" s="28" t="s">
         <v>40</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" ht="30" customHeight="1">
       <c r="B40" s="28" t="s">
         <v>41</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" ht="30" customHeight="1">
       <c r="B41" s="28" t="s">
         <v>42</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="30" customHeight="1">
       <c r="B42" s="32" t="s">
         <v>17</v>
       </c>
@@ -2228,7 +2228,7 @@
       <c r="F42" s="32"/>
       <c r="G42" s="35"/>
     </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" ht="30" customHeight="1">
       <c r="B43" s="28" t="s">
         <v>20</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="30" customHeight="1">
       <c r="B44" s="28" t="s">
         <v>18</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" ht="30" customHeight="1">
       <c r="B45" s="28" t="s">
         <v>19</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="30" customHeight="1">
       <c r="B46" s="33" t="s">
         <v>21</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="F46" s="33"/>
       <c r="G46" s="39"/>
     </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" ht="30" customHeight="1">
       <c r="B47" s="28" t="s">
         <v>22</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" ht="30" customHeight="1">
       <c r="B48" s="28" t="s">
         <v>23</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="30" customHeight="1">
       <c r="B49" s="34" t="s">
         <v>24</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="F49" s="34"/>
       <c r="G49" s="46"/>
     </row>
-    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" ht="30" customHeight="1">
       <c r="B50" s="28" t="s">
         <v>25</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" ht="30" customHeight="1">
       <c r="B51" s="28" t="s">
         <v>26</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" ht="30" customHeight="1">
       <c r="B52" s="28" t="s">
         <v>27</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7" ht="30" customHeight="1">
       <c r="B53" s="28" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
docs(GANTT): update gantt chart
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C07E049D-7210-4BC1-8A06-9A03FFD2ACFA}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{10280783-3C1E-9342-A19E-03A845D378D4}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3560" yWindow="460" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -326,12 +326,16 @@
     <t>3.21 Correctness proof</t>
     <phoneticPr fontId="16" type="noConversion"/>
   </si>
+  <si>
+    <t>3.22 Refactor &amp; documen</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -878,20 +882,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1280,13 +1284,13 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AM53"/>
+  <dimension ref="B1:AM54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="61" zoomScaleNormal="61" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BK26" sqref="BK26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="61" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
@@ -1296,7 +1300,7 @@
     <col min="28" max="67" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1">
+    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="12" t="s">
         <v>38</v>
       </c>
@@ -1306,7 +1310,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1">
+    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="50" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1364,7 @@
       <c r="AL2" s="21"/>
       <c r="AM2" s="21"/>
     </row>
-    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1">
+    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1428,7 @@
       <c r="AH3" s="49"/>
       <c r="AI3" s="49"/>
     </row>
-    <row r="4" spans="2:39" ht="15.75" customHeight="1">
+    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="52"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -1516,7 +1520,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="30" customHeight="1">
+    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:39" ht="30" customHeight="1">
+    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="30" customHeight="1">
+    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
         <v>30</v>
       </c>
@@ -1576,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="30" customHeight="1">
+    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -1596,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="30" customHeight="1">
+    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -1616,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="30" customHeight="1">
+    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
@@ -1636,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1">
+    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="30" customHeight="1">
+    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="28" t="s">
         <v>34</v>
       </c>
@@ -1676,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:39" ht="30" customHeight="1">
+    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>35</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="30" customHeight="1">
+    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="28" t="s">
         <v>36</v>
       </c>
@@ -1716,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="30" customHeight="1">
+    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="28" t="s">
         <v>37</v>
       </c>
@@ -1736,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="30" customHeight="1">
+    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
         <v>15</v>
       </c>
@@ -1752,7 +1756,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="36"/>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
@@ -1772,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="s">
         <v>48</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="28" t="s">
         <v>47</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="28" t="s">
         <v>45</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="28" t="s">
         <v>43</v>
       </c>
@@ -1852,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>44</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>46</v>
       </c>
@@ -1892,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>49</v>
       </c>
@@ -1912,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="28" t="s">
         <v>50</v>
       </c>
@@ -1932,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="28" t="s">
         <v>51</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="28" t="s">
         <v>52</v>
       </c>
@@ -1972,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="28" t="s">
         <v>53</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="28" t="s">
         <v>54</v>
       </c>
@@ -2012,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="28" t="s">
         <v>55</v>
       </c>
@@ -2032,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="28" t="s">
         <v>56</v>
       </c>
@@ -2045,12 +2049,14 @@
       <c r="E31" s="6">
         <v>21</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="6">
+        <v>3</v>
+      </c>
       <c r="G31" s="7">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="28" t="s">
         <v>57</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="28" t="s">
         <v>58</v>
       </c>
@@ -2088,7 +2094,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="28" t="s">
         <v>59</v>
       </c>
@@ -2101,12 +2107,14 @@
       <c r="E34" s="6">
         <v>23</v>
       </c>
-      <c r="F34" s="6"/>
+      <c r="F34" s="6">
+        <v>2</v>
+      </c>
       <c r="G34" s="7">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="28" t="s">
         <v>60</v>
       </c>
@@ -2119,10 +2127,14 @@
       <c r="E35" s="6">
         <v>24</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1">
+      <c r="F35" s="6">
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="28" t="s">
         <v>61</v>
       </c>
@@ -2135,10 +2147,14 @@
       <c r="E36" s="6">
         <v>24</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1">
+      <c r="F36" s="6">
+        <v>1</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="28" t="s">
         <v>62</v>
       </c>
@@ -2148,50 +2164,51 @@
       <c r="D37" s="6">
         <v>1</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1">
+      <c r="E37" s="6">
+        <v>24</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="6">
+        <v>25</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="6">
-        <v>21</v>
-      </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <v>3</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6">
+      <c r="E39" s="6"/>
+      <c r="F39" s="6">
         <v>2</v>
       </c>
-      <c r="G38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1">
-      <c r="B39" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="6">
-        <v>19</v>
-      </c>
-      <c r="D39" s="6">
-        <v>2</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
       <c r="G39" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1">
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="6">
         <v>2</v>
@@ -2202,15 +2219,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="30" customHeight="1">
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -2218,106 +2235,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1">
-      <c r="B42" s="32" t="s">
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="6">
+        <v>21</v>
+      </c>
+      <c r="D42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="35"/>
-    </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1">
-      <c r="B43" s="28" t="s">
+      <c r="C43" s="35"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="35"/>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C44" s="6">
         <v>5</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <v>4</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E44" s="6">
         <v>5</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F44" s="6">
         <v>5</v>
       </c>
-      <c r="G43" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="30" customHeight="1">
-      <c r="B44" s="28" t="s">
+      <c r="G44" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="28" t="s">
         <v>18</v>
-      </c>
-      <c r="C44" s="6">
-        <v>22</v>
-      </c>
-      <c r="D44" s="6">
-        <v>6</v>
-      </c>
-      <c r="E44" s="6">
-        <v>22</v>
-      </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1">
-      <c r="B45" s="28" t="s">
-        <v>19</v>
       </c>
       <c r="C45" s="6">
         <v>22</v>
       </c>
       <c r="D45" s="6">
-        <v>7</v>
-      </c>
-      <c r="E45" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="E45" s="6">
+        <v>22</v>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="6">
+        <v>22</v>
+      </c>
+      <c r="D46" s="6">
+        <v>7</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:7" ht="30" customHeight="1">
-      <c r="B46" s="33" t="s">
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="39">
+      <c r="C47" s="39">
         <v>21</v>
       </c>
-      <c r="D46" s="39">
+      <c r="D47" s="39">
         <v>6</v>
       </c>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="39"/>
-    </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1">
-      <c r="B47" s="28" t="s">
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="39"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C48" s="6">
         <v>21</v>
-      </c>
-      <c r="D47" s="6">
-        <v>3</v>
-      </c>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="30" customHeight="1">
-      <c r="B48" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="6">
-        <v>24</v>
       </c>
       <c r="D48" s="6">
         <v>3</v>
@@ -2328,42 +2345,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1">
-      <c r="B49" s="34" t="s">
+    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="6">
         <v>24</v>
       </c>
-      <c r="C49" s="40">
+      <c r="D49" s="6">
+        <v>3</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="40">
         <v>21</v>
       </c>
-      <c r="D49" s="40">
+      <c r="D50" s="40">
         <v>8</v>
       </c>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="46"/>
-    </row>
-    <row r="50" spans="2:7" ht="30" customHeight="1">
-      <c r="B50" s="28" t="s">
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="46"/>
+    </row>
+    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C51" s="6">
         <v>21</v>
-      </c>
-      <c r="D50" s="6">
-        <v>3</v>
-      </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" ht="30" customHeight="1">
-      <c r="B51" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="6">
-        <v>23</v>
       </c>
       <c r="D51" s="6">
         <v>3</v>
@@ -2374,12 +2391,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="30" customHeight="1">
+    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C52" s="6">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D52" s="6">
         <v>3</v>
@@ -2390,19 +2407,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30" customHeight="1">
+    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C53" s="6">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D53" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E53" s="28"/>
       <c r="F53" s="28"/>
       <c r="G53" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="6">
+        <v>28</v>
+      </c>
+      <c r="D54" s="6">
+        <v>1</v>
+      </c>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="45">
         <v>0</v>
       </c>
     </row>
@@ -2426,7 +2459,7 @@
     <mergeCell ref="J3:K3"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
-  <conditionalFormatting sqref="H5:AI53">
+  <conditionalFormatting sqref="H5:AI54">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2452,7 +2485,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:BO54">
+  <conditionalFormatting sqref="B55:BO55">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs(minutes): add 39th meeting
</commit_message>
<xml_diff>
--- a/GANTT_new.xlsx
+++ b/GANTT_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/791c94ee7340d2cd/Doc/Uni-S5/1-Software Engineering Group Project 2043/PublicFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{10280783-3C1E-9342-A19E-03A845D378D4}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{16CFD1E7-8441-344C-AF3D-E3A5AA056977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E8D8D7B8-2796-473A-9E2A-BED480CD95B5}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="460" windowWidth="37700" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="830" yWindow="-110" windowWidth="37680" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -882,20 +882,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="标题" xfId="8" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1286,11 +1286,11 @@
   </sheetPr>
   <dimension ref="B1:AM54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="61" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BG13" sqref="BG13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" style="2" customWidth="1"/>
@@ -1300,7 +1300,7 @@
     <col min="28" max="67" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:39" ht="60" customHeight="1" thickBot="1">
       <c r="B1" s="12" t="s">
         <v>38</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:39" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="B2" s="50" t="s">
         <v>4</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="13">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="57" t="s">
@@ -1364,7 +1364,7 @@
       <c r="AL2" s="21"/>
       <c r="AM2" s="21"/>
     </row>
-    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:39" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1">
       <c r="B3" s="51" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="AH3" s="49"/>
       <c r="AI3" s="49"/>
     </row>
-    <row r="4" spans="2:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:39" ht="15.75" customHeight="1">
       <c r="B4" s="52"/>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -1520,7 +1520,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:39" ht="30" customHeight="1">
       <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:39" ht="30" customHeight="1">
       <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:39" ht="30" customHeight="1">
       <c r="B7" s="28" t="s">
         <v>30</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:39" ht="30" customHeight="1">
       <c r="B8" s="28" t="s">
         <v>31</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:39" ht="30" customHeight="1">
       <c r="B9" s="28" t="s">
         <v>32</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:39" ht="30" customHeight="1">
       <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:39" ht="30" customHeight="1">
       <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:39" ht="30" customHeight="1">
       <c r="B12" s="28" t="s">
         <v>34</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:39" ht="30" customHeight="1">
       <c r="B13" s="28" t="s">
         <v>35</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:39" ht="30" customHeight="1">
       <c r="B14" s="28" t="s">
         <v>36</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:39" ht="30" customHeight="1">
       <c r="B15" s="28" t="s">
         <v>37</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:39" ht="30" customHeight="1">
       <c r="B16" s="31" t="s">
         <v>15</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="F16" s="31"/>
       <c r="G16" s="36"/>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="30" customHeight="1">
       <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="30" customHeight="1">
       <c r="B18" s="28" t="s">
         <v>48</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="30" customHeight="1">
       <c r="B19" s="28" t="s">
         <v>47</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="30" customHeight="1">
       <c r="B20" s="28" t="s">
         <v>45</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="30" customHeight="1">
       <c r="B21" s="28" t="s">
         <v>43</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="30" customHeight="1">
       <c r="B22" s="28" t="s">
         <v>44</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="30" customHeight="1">
       <c r="B23" s="28" t="s">
         <v>46</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="28" t="s">
         <v>49</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="30" customHeight="1">
       <c r="B25" s="28" t="s">
         <v>50</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="30" customHeight="1">
       <c r="B26" s="28" t="s">
         <v>51</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="30" customHeight="1">
       <c r="B27" s="28" t="s">
         <v>52</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="30" customHeight="1">
       <c r="B28" s="28" t="s">
         <v>53</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="30" customHeight="1">
       <c r="B29" s="28" t="s">
         <v>54</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" ht="30" customHeight="1">
       <c r="B30" s="28" t="s">
         <v>55</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" ht="30" customHeight="1">
       <c r="B31" s="28" t="s">
         <v>56</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" ht="30" customHeight="1">
       <c r="B32" s="28" t="s">
         <v>57</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="30" customHeight="1">
       <c r="B33" s="28" t="s">
         <v>58</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" ht="30" customHeight="1">
       <c r="B34" s="28" t="s">
         <v>59</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" ht="30" customHeight="1">
       <c r="B35" s="28" t="s">
         <v>60</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" ht="30" customHeight="1">
       <c r="B36" s="28" t="s">
         <v>61</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" ht="30" customHeight="1">
       <c r="B37" s="28" t="s">
         <v>62</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="30" customHeight="1">
       <c r="B38" s="28" t="s">
         <v>63</v>
       </c>
@@ -2188,7 +2188,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="30" customHeight="1">
       <c r="B39" s="28" t="s">
         <v>39</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" ht="30" customHeight="1">
       <c r="B40" s="28" t="s">
         <v>40</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" ht="30" customHeight="1">
       <c r="B41" s="28" t="s">
         <v>41</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" ht="30" customHeight="1">
       <c r="B42" s="28" t="s">
         <v>42</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="30" customHeight="1">
       <c r="B43" s="32" t="s">
         <v>17</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="F43" s="32"/>
       <c r="G43" s="35"/>
     </row>
-    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="30" customHeight="1">
       <c r="B44" s="28" t="s">
         <v>20</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" ht="30" customHeight="1">
       <c r="B45" s="28" t="s">
         <v>18</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" ht="30" customHeight="1">
       <c r="B46" s="28" t="s">
         <v>19</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="30" customHeight="1">
       <c r="B47" s="33" t="s">
         <v>21</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="F47" s="33"/>
       <c r="G47" s="39"/>
     </row>
-    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" ht="30" customHeight="1">
       <c r="B48" s="28" t="s">
         <v>22</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7" ht="30" customHeight="1">
       <c r="B49" s="28" t="s">
         <v>23</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="30" customHeight="1">
       <c r="B50" s="34" t="s">
         <v>24</v>
       </c>
@@ -2375,7 +2375,7 @@
       <c r="F50" s="34"/>
       <c r="G50" s="46"/>
     </row>
-    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" ht="30" customHeight="1">
       <c r="B51" s="28" t="s">
         <v>25</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" ht="30" customHeight="1">
       <c r="B52" s="28" t="s">
         <v>26</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7" ht="30" customHeight="1">
       <c r="B53" s="28" t="s">
         <v>27</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:7" ht="30" customHeight="1">
       <c r="B54" s="28" t="s">
         <v>28</v>
       </c>

</xml_diff>